<commit_message>
CCO CDO 2024 corrected - RP3 methodology
</commit_message>
<xml_diff>
--- a/static/download/2024/RP3_APT_CDO_2024_Jan_Dec.xlsx
+++ b/static/download/2024/RP3_APT_CDO_2024_Jan_Dec.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="341">
   <si>
     <t>Data source</t>
   </si>
@@ -935,6 +935,9 @@
     <t>LPFL</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Faro (LPFR)</t>
   </si>
   <si>
@@ -1026,6 +1029,12 @@
   </si>
   <si>
     <t>UK airports removed</t>
+  </si>
+  <si>
+    <t>all apts</t>
+  </si>
+  <si>
+    <t>file updated with slightly revised figures to align with RP3 methodology</t>
   </si>
 </sst>
 </file>
@@ -1279,6 +1288,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="17" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1287,9 +1299,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1353,7 +1362,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="6">
-        <v>45758.0</v>
+        <v>45828.0</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>6</v>
@@ -1436,10 +1445,11 @@
         <v>96625.0</v>
       </c>
       <c r="E6" s="21">
-        <v>14821.0</v>
+        <v>16889.0</v>
       </c>
       <c r="F6" s="22">
-        <v>0.153</v>
+        <f t="shared" ref="F6:F55" si="1">E6/D6</f>
+        <v>0.1747891332</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -1456,10 +1466,11 @@
         <v>94212.0</v>
       </c>
       <c r="E7" s="21">
-        <v>16890.0</v>
+        <v>21874.0</v>
       </c>
       <c r="F7" s="22">
-        <v>0.179</v>
+        <f t="shared" si="1"/>
+        <v>0.2321784911</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
@@ -1476,10 +1487,11 @@
         <v>5589.0</v>
       </c>
       <c r="E8" s="21">
-        <v>1248.0</v>
+        <v>1306.0</v>
       </c>
       <c r="F8" s="22">
-        <v>0.223</v>
+        <f t="shared" si="1"/>
+        <v>0.2336732868</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
@@ -1496,10 +1508,11 @@
         <v>1359.0</v>
       </c>
       <c r="E9" s="21">
-        <v>186.0</v>
+        <v>211.0</v>
       </c>
       <c r="F9" s="22">
-        <v>0.137</v>
+        <f t="shared" si="1"/>
+        <v>0.1552612215</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
@@ -1516,10 +1529,11 @@
         <v>219497.0</v>
       </c>
       <c r="E10" s="21">
-        <v>8714.0</v>
+        <v>9721.0</v>
       </c>
       <c r="F10" s="22">
-        <v>0.04</v>
+        <f t="shared" si="1"/>
+        <v>0.04428762124</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
@@ -1536,10 +1550,11 @@
         <v>8285.0</v>
       </c>
       <c r="E11" s="21">
-        <v>1619.0</v>
+        <v>1920.0</v>
       </c>
       <c r="F11" s="22">
-        <v>0.195</v>
+        <f t="shared" si="1"/>
+        <v>0.2317441159</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
@@ -1556,10 +1571,11 @@
         <v>60170.0</v>
       </c>
       <c r="E12" s="21">
-        <v>13632.0</v>
+        <v>17147.0</v>
       </c>
       <c r="F12" s="22">
-        <v>0.227</v>
+        <f t="shared" si="1"/>
+        <v>0.2849759016</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
@@ -1576,10 +1592,11 @@
         <v>56854.0</v>
       </c>
       <c r="E13" s="21">
-        <v>10702.0</v>
+        <v>10445.0</v>
       </c>
       <c r="F13" s="22">
-        <v>0.188</v>
+        <f t="shared" si="1"/>
+        <v>0.1837161853</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
@@ -1596,10 +1613,11 @@
         <v>77265.0</v>
       </c>
       <c r="E14" s="21">
-        <v>13444.0</v>
+        <v>14201.0</v>
       </c>
       <c r="F14" s="22">
-        <v>0.174</v>
+        <f t="shared" si="1"/>
+        <v>0.1837960267</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
@@ -1616,10 +1634,11 @@
         <v>161547.0</v>
       </c>
       <c r="E15" s="21">
-        <v>7033.0</v>
+        <v>8182.0</v>
       </c>
       <c r="F15" s="22">
-        <v>0.044</v>
+        <f t="shared" si="1"/>
+        <v>0.05064779909</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
@@ -1636,10 +1655,11 @@
         <v>18870.0</v>
       </c>
       <c r="E16" s="21">
-        <v>2429.0</v>
+        <v>2362.0</v>
       </c>
       <c r="F16" s="22">
-        <v>0.129</v>
+        <f t="shared" si="1"/>
+        <v>0.1251722311</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
@@ -1656,10 +1676,11 @@
         <v>36063.0</v>
       </c>
       <c r="E17" s="21">
-        <v>4778.0</v>
+        <v>5742.0</v>
       </c>
       <c r="F17" s="22">
-        <v>0.132</v>
+        <f t="shared" si="1"/>
+        <v>0.1592213626</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
@@ -1676,10 +1697,11 @@
         <v>2460.0</v>
       </c>
       <c r="E18" s="21">
-        <v>297.0</v>
+        <v>290.0</v>
       </c>
       <c r="F18" s="22">
-        <v>0.121</v>
+        <f t="shared" si="1"/>
+        <v>0.1178861789</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
@@ -1696,10 +1718,11 @@
         <v>41985.0</v>
       </c>
       <c r="E19" s="21">
-        <v>3621.0</v>
+        <v>3897.0</v>
       </c>
       <c r="F19" s="22">
-        <v>0.086</v>
+        <f t="shared" si="1"/>
+        <v>0.09281886388</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
@@ -1716,10 +1739,11 @@
         <v>24453.0</v>
       </c>
       <c r="E20" s="21">
-        <v>5716.0</v>
+        <v>6358.0</v>
       </c>
       <c r="F20" s="22">
-        <v>0.234</v>
+        <f t="shared" si="1"/>
+        <v>0.2600089969</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
@@ -1736,10 +1760,11 @@
         <v>10517.0</v>
       </c>
       <c r="E21" s="21">
-        <v>2183.0</v>
+        <v>2410.0</v>
       </c>
       <c r="F21" s="22">
-        <v>0.208</v>
+        <f t="shared" si="1"/>
+        <v>0.2291528002</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
@@ -1759,7 +1784,8 @@
         <v>13272.0</v>
       </c>
       <c r="F22" s="22">
-        <v>0.692</v>
+        <f t="shared" si="1"/>
+        <v>0.6922956549</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
@@ -1779,7 +1805,8 @@
         <v>400.0</v>
       </c>
       <c r="F23" s="22">
-        <v>0.778</v>
+        <f t="shared" si="1"/>
+        <v>0.7782101167</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
@@ -1799,7 +1826,8 @@
         <v>47827.0</v>
       </c>
       <c r="F24" s="22">
-        <v>0.627</v>
+        <f t="shared" si="1"/>
+        <v>0.6273874488</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
@@ -1819,7 +1847,8 @@
         <v>60549.0</v>
       </c>
       <c r="F25" s="22">
-        <v>0.249</v>
+        <f t="shared" si="1"/>
+        <v>0.2486142248</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
@@ -1839,7 +1868,8 @@
         <v>396.0</v>
       </c>
       <c r="F26" s="22">
-        <v>0.131</v>
+        <f t="shared" si="1"/>
+        <v>0.1309956996</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
@@ -1859,7 +1889,8 @@
         <v>647.0</v>
       </c>
       <c r="F27" s="22">
-        <v>0.24</v>
+        <f t="shared" si="1"/>
+        <v>0.2403417533</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
@@ -1879,7 +1910,8 @@
         <v>2260.0</v>
       </c>
       <c r="F28" s="22">
-        <v>0.19</v>
+        <f t="shared" si="1"/>
+        <v>0.1904761905</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
@@ -1899,7 +1931,8 @@
         <v>5795.0</v>
       </c>
       <c r="F29" s="22">
-        <v>0.517</v>
+        <f t="shared" si="1"/>
+        <v>0.517041399</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
@@ -1919,7 +1952,8 @@
         <v>48420.0</v>
       </c>
       <c r="F30" s="22">
-        <v>0.399</v>
+        <f t="shared" si="1"/>
+        <v>0.3989913972</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
@@ -1939,7 +1973,8 @@
         <v>5481.0</v>
       </c>
       <c r="F31" s="22">
-        <v>0.511</v>
+        <f t="shared" si="1"/>
+        <v>0.5107632094</v>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
@@ -1959,7 +1994,8 @@
         <v>58221.0</v>
       </c>
       <c r="F32" s="22">
-        <v>0.486</v>
+        <f t="shared" si="1"/>
+        <v>0.4855148604</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
@@ -1979,7 +2015,8 @@
         <v>12714.0</v>
       </c>
       <c r="F33" s="22">
-        <v>0.357</v>
+        <f t="shared" si="1"/>
+        <v>0.3565339316</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
@@ -1999,7 +2036,8 @@
         <v>31728.0</v>
       </c>
       <c r="F34" s="22">
-        <v>0.738</v>
+        <f t="shared" si="1"/>
+        <v>0.7377232143</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
@@ -2019,7 +2057,8 @@
         <v>64002.0</v>
       </c>
       <c r="F35" s="22">
-        <v>0.586</v>
+        <f t="shared" si="1"/>
+        <v>0.5860184041</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
@@ -2039,7 +2078,8 @@
         <v>19973.0</v>
       </c>
       <c r="F36" s="22">
-        <v>0.784</v>
+        <f t="shared" si="1"/>
+        <v>0.784115892</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
@@ -2059,7 +2099,8 @@
         <v>19302.0</v>
       </c>
       <c r="F37" s="22">
-        <v>0.703</v>
+        <f t="shared" si="1"/>
+        <v>0.7031693989</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
@@ -2079,7 +2120,8 @@
         <v>706.0</v>
       </c>
       <c r="F38" s="22">
-        <v>0.376</v>
+        <f t="shared" si="1"/>
+        <v>0.3755319149</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
@@ -2099,7 +2141,8 @@
         <v>13604.0</v>
       </c>
       <c r="F39" s="22">
-        <v>0.534</v>
+        <f t="shared" si="1"/>
+        <v>0.5339927775</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
@@ -2119,7 +2162,8 @@
         <v>16977.0</v>
       </c>
       <c r="F40" s="22">
-        <v>0.452</v>
+        <f t="shared" si="1"/>
+        <v>0.4515399755</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
@@ -2139,7 +2183,8 @@
         <v>8049.0</v>
       </c>
       <c r="F41" s="22">
-        <v>0.364</v>
+        <f t="shared" si="1"/>
+        <v>0.3636979802</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
@@ -2159,7 +2204,8 @@
         <v>747.0</v>
       </c>
       <c r="F42" s="22">
-        <v>0.435</v>
+        <f t="shared" si="1"/>
+        <v>0.4348079162</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
@@ -2179,7 +2225,8 @@
         <v>765.0</v>
       </c>
       <c r="F43" s="22">
-        <v>0.489</v>
+        <f t="shared" si="1"/>
+        <v>0.4891304348</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
@@ -2199,7 +2246,8 @@
         <v>5131.0</v>
       </c>
       <c r="F44" s="22">
-        <v>0.621</v>
+        <f t="shared" si="1"/>
+        <v>0.6207355432</v>
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
@@ -2219,7 +2267,8 @@
         <v>5001.0</v>
       </c>
       <c r="F45" s="22">
-        <v>0.349</v>
+        <f t="shared" si="1"/>
+        <v>0.3485017422</v>
       </c>
     </row>
     <row r="46" ht="12.75" customHeight="1">
@@ -2239,7 +2288,8 @@
         <v>113.0</v>
       </c>
       <c r="F46" s="22">
-        <v>0.219</v>
+        <f t="shared" si="1"/>
+        <v>0.2185686654</v>
       </c>
     </row>
     <row r="47" ht="12.75" customHeight="1">
@@ -2259,7 +2309,8 @@
         <v>2596.0</v>
       </c>
       <c r="F47" s="22">
-        <v>0.338</v>
+        <f t="shared" si="1"/>
+        <v>0.3376251788</v>
       </c>
     </row>
     <row r="48" ht="12.75" customHeight="1">
@@ -2279,7 +2330,8 @@
         <v>1345.0</v>
       </c>
       <c r="F48" s="22">
-        <v>0.532</v>
+        <f t="shared" si="1"/>
+        <v>0.5324623911</v>
       </c>
     </row>
     <row r="49" ht="12.75" customHeight="1">
@@ -2299,7 +2351,8 @@
         <v>216.0</v>
       </c>
       <c r="F49" s="22">
-        <v>0.405</v>
+        <f t="shared" si="1"/>
+        <v>0.4052532833</v>
       </c>
     </row>
     <row r="50" ht="12.75" customHeight="1">
@@ -2319,7 +2372,8 @@
         <v>41989.0</v>
       </c>
       <c r="F50" s="22">
-        <v>0.462</v>
+        <f t="shared" si="1"/>
+        <v>0.4619455202</v>
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
@@ -2339,7 +2393,8 @@
         <v>5468.0</v>
       </c>
       <c r="F51" s="22">
-        <v>0.303</v>
+        <f t="shared" si="1"/>
+        <v>0.3034406215</v>
       </c>
     </row>
     <row r="52" ht="12.75" customHeight="1">
@@ -2359,7 +2414,8 @@
         <v>211.0</v>
       </c>
       <c r="F52" s="22">
-        <v>0.349</v>
+        <f t="shared" si="1"/>
+        <v>0.3493377483</v>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
@@ -2379,7 +2435,8 @@
         <v>46201.0</v>
       </c>
       <c r="F53" s="22">
-        <v>0.487</v>
+        <f t="shared" si="1"/>
+        <v>0.4868028702</v>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
@@ -2399,7 +2456,8 @@
         <v>23.0</v>
       </c>
       <c r="F54" s="22">
-        <v>0.442</v>
+        <f t="shared" si="1"/>
+        <v>0.4423076923</v>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
@@ -2419,7 +2477,8 @@
         <v>18182.0</v>
       </c>
       <c r="F55" s="22">
-        <v>0.633</v>
+        <f t="shared" si="1"/>
+        <v>0.632681467</v>
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
@@ -2432,8 +2491,12 @@
       <c r="C56" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
+      <c r="D56" s="21">
+        <v>6.0</v>
+      </c>
+      <c r="E56" s="21">
+        <v>4.0</v>
+      </c>
       <c r="F56" s="22"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
@@ -4086,16 +4149,20 @@
       <c r="C139" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="D139" s="21"/>
-      <c r="E139" s="21"/>
+      <c r="D139" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="E139" s="21" t="s">
+        <v>307</v>
+      </c>
       <c r="F139" s="22"/>
     </row>
     <row r="140" ht="12.75" customHeight="1">
       <c r="A140" s="19" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B140" s="19" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C140" s="20" t="s">
         <v>302</v>
@@ -4112,10 +4179,10 @@
     </row>
     <row r="141" ht="12.75" customHeight="1">
       <c r="A141" s="19" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B141" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C141" s="20" t="s">
         <v>302</v>
@@ -4132,10 +4199,10 @@
     </row>
     <row r="142" ht="12.75" customHeight="1">
       <c r="A142" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C142" s="20" t="s">
         <v>302</v>
@@ -4152,10 +4219,10 @@
     </row>
     <row r="143" ht="12.75" customHeight="1">
       <c r="A143" s="19" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B143" s="19" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C143" s="20" t="s">
         <v>302</v>
@@ -4172,10 +4239,10 @@
     </row>
     <row r="144" ht="12.75" customHeight="1">
       <c r="A144" s="19" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B144" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C144" s="20" t="s">
         <v>302</v>
@@ -4192,10 +4259,10 @@
     </row>
     <row r="145" ht="12.75" customHeight="1">
       <c r="A145" s="19" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C145" s="20" t="s">
         <v>302</v>
@@ -4212,10 +4279,10 @@
     </row>
     <row r="146" ht="12.75" customHeight="1">
       <c r="A146" s="19" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B146" s="19" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C146" s="20" t="s">
         <v>302</v>
@@ -4232,13 +4299,13 @@
     </row>
     <row r="147" ht="12.75" customHeight="1">
       <c r="A147" s="19" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B147" s="19" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C147" s="20" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D147" s="21">
         <v>2367.0</v>
@@ -4252,13 +4319,13 @@
     </row>
     <row r="148" ht="12.75" customHeight="1">
       <c r="A148" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="B148" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="C148" s="20" t="s">
         <v>324</v>
-      </c>
-      <c r="B148" s="19" t="s">
-        <v>325</v>
-      </c>
-      <c r="C148" s="20" t="s">
-        <v>323</v>
       </c>
       <c r="D148" s="21">
         <v>58250.0</v>
@@ -4272,13 +4339,13 @@
     </row>
     <row r="149" ht="12.75" customHeight="1">
       <c r="A149" s="19" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B149" s="19" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C149" s="20" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D149" s="21">
         <v>85990.0</v>
@@ -4292,13 +4359,13 @@
     </row>
     <row r="150" ht="12.75" customHeight="1">
       <c r="A150" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="B150" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="C150" s="20" t="s">
         <v>329</v>
-      </c>
-      <c r="B150" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="C150" s="20" t="s">
-        <v>328</v>
       </c>
       <c r="D150" s="21">
         <v>128483.0</v>
@@ -4339,16 +4406,16 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -4362,7 +4429,7 @@
         <v>2021.0</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
@@ -4370,24 +4437,32 @@
         <v>44351.0</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="29" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="25"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33"/>
+      <c r="A4" s="28">
+        <v>45828.0</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="27">
+        <v>2024.0</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="34"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>